<commit_message>
desde work 28 May para server
</commit_message>
<xml_diff>
--- a/src/assets/plantilla.xlsx
+++ b/src/assets/plantilla.xlsx
@@ -193,19 +193,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,9 +292,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1242720</xdr:colOff>
+      <xdr:colOff>1242360</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -308,7 +308,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="392760" y="10080"/>
-          <a:ext cx="1183320" cy="1111680"/>
+          <a:ext cx="1182960" cy="1111320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -503,7 +503,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -564,6 +564,7 @@
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="8.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="4"/>
@@ -595,11 +596,12 @@
       <c r="J8" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.590277777777778" right="0.590277777777778" top="0.590277777777778" bottom="0.590277777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Desde work 11 Jul
</commit_message>
<xml_diff>
--- a/src/assets/plantilla.xlsx
+++ b/src/assets/plantilla.xlsx
@@ -292,9 +292,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1242360</xdr:colOff>
+      <xdr:colOff>1241280</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:rowOff>5400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -308,7 +308,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="392760" y="10080"/>
-          <a:ext cx="1182960" cy="1111320"/>
+          <a:ext cx="1181880" cy="1110240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -500,10 +500,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -517,8 +517,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.39"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="1" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.39"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="13" style="1" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -534,6 +536,8 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C2" s="3" t="s">
@@ -563,8 +567,8 @@
         <v>4</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="8.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="4"/>
@@ -582,6 +586,8 @@
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
@@ -593,11 +599,13 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="C4:D4"/>

</xml_diff>

<commit_message>
desde work 17 Julio
</commit_message>
<xml_diff>
--- a/src/assets/plantilla.xlsx
+++ b/src/assets/plantilla.xlsx
@@ -19,10 +19,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="J7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[días]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[días]</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t xml:space="preserve">REPORTE GENERAL PLANTA BAJA</t>
+    <t xml:space="preserve">TITULO REPORTE </t>
   </si>
   <si>
     <t xml:space="preserve">Rango de Fechas:</t>
@@ -44,7 +78,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -99,6 +133,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -156,12 +195,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,9 +335,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1241280</xdr:colOff>
+      <xdr:colOff>1238760</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>5400</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -308,7 +351,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="392760" y="10080"/>
-          <a:ext cx="1181880" cy="1110240"/>
+          <a:ext cx="1179360" cy="1107720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -503,112 +546,115 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.1"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.74"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="13" style="1" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="8.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C6" s="4"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="24.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="12"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:L1"/>
+  <mergeCells count="6">
+    <mergeCell ref="C1:L1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
     <mergeCell ref="E5:F5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -618,6 +664,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
desde work 18 Julio para server
</commit_message>
<xml_diff>
--- a/src/assets/plantilla.xlsx
+++ b/src/assets/plantilla.xlsx
@@ -335,9 +335,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1238760</xdr:colOff>
+      <xdr:colOff>1238040</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>2160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -351,7 +351,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="392760" y="10080"/>
-          <a:ext cx="1179360" cy="1107720"/>
+          <a:ext cx="1178640" cy="1107000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -546,13 +546,13 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.61"/>

</xml_diff>

<commit_message>
desde work 16 Dic
</commit_message>
<xml_diff>
--- a/src/assets/plantilla.xlsx
+++ b/src/assets/plantilla.xlsx
@@ -296,9 +296,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1237680</xdr:colOff>
+      <xdr:colOff>1237320</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1800</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -312,7 +312,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="392760" y="10080"/>
-          <a:ext cx="1178280" cy="1106640"/>
+          <a:ext cx="1177920" cy="1106280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -504,13 +504,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="11.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.33"/>
@@ -520,13 +520,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="6.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="7.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18.74"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="15" style="1" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="15" style="1" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -545,7 +545,6 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C2" s="4" t="s">
@@ -556,7 +555,6 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C3" s="6" t="s">
@@ -574,7 +572,6 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C5" s="4" t="s">
@@ -603,7 +600,6 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10"/>
@@ -618,12 +614,11 @@
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="13"/>
+      <c r="M8" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="C1:M1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="C4:D4"/>

</xml_diff>